<commit_message>
use storage Bucket instead of local files
</commit_message>
<xml_diff>
--- a/DataTemplates/Config.xlsx
+++ b/DataTemplates/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmad\Desktop\Nuummite starter templete\NuummiteUipathTemplate\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmad\Documents\UiPath\NuummiteUipathTemplate\DataTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="15" windowWidth="10935" windowHeight="8190"/>
+    <workbookView xWindow="5610" yWindow="15" windowWidth="10935" windowHeight="8190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Orchestrator Folder</t>
   </si>
   <si>
-    <t>HistoryFilePath</t>
-  </si>
-  <si>
     <t>ProcessNickName</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Additional sub folders will be created under this on every run by robot to store temporary files and exception screen shots.</t>
   </si>
   <si>
-    <t>This file will be used to log start time,end time,temporary folder path and status on every run</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
   </si>
   <si>
     <t>E:\temp</t>
-  </si>
-  <si>
-    <t>E:\History.xlsx</t>
   </si>
   <si>
     <t>Bot_SMTP_MailServer</t>
@@ -559,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -578,106 +569,106 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>465</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>993</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -688,10 +679,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,72 +711,61 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -818,13 +798,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -855,30 +835,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete some values from the config file
</commit_message>
<xml_diff>
--- a/DataTemplates/Config.xlsx
+++ b/DataTemplates/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="15" windowWidth="10935" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="5610" yWindow="15" windowWidth="10935" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -95,39 +95,6 @@
     <t>E:\temp</t>
   </si>
   <si>
-    <t>Bot_SMTP_MailServer</t>
-  </si>
-  <si>
-    <t>smtp mail server for send emails</t>
-  </si>
-  <si>
-    <t>Bot_SMTP_MailPort</t>
-  </si>
-  <si>
-    <t>smtp mail port for send emails</t>
-  </si>
-  <si>
-    <t>Bot_IMAP_MailServer</t>
-  </si>
-  <si>
-    <t>smtp mail server for receive emails</t>
-  </si>
-  <si>
-    <t>Bot_IMAP_MailPort</t>
-  </si>
-  <si>
-    <t>smtp mail port for receive emails</t>
-  </si>
-  <si>
-    <t>BotMailProtocol</t>
-  </si>
-  <si>
-    <t>imap&amp;smtp</t>
-  </si>
-  <si>
-    <t>mail prtocol of bot for send and receive emails</t>
-  </si>
-  <si>
     <t>BotEmail</t>
   </si>
   <si>
@@ -147,12 +114,6 @@
   </si>
   <si>
     <t>email body for  business exceptions</t>
-  </si>
-  <si>
-    <t>imap.gmail.com</t>
-  </si>
-  <si>
-    <t>smtp.gmail.com</t>
   </si>
   <si>
     <t>Asset Name</t>
@@ -548,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,98 +538,43 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>465</v>
+        <v>26</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B6">
-        <v>993</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -681,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -730,7 +636,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -798,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -849,16 +755,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>